<commit_message>
feat: comparision with STANDING Together recommendations
</commit_message>
<xml_diff>
--- a/outputs/metadata_elements_comparison_matrix.xlsx
+++ b/outputs/metadata_elements_comparison_matrix.xlsx
@@ -465,81 +465,81 @@
         <v>100</v>
       </c>
       <c r="B2" t="n">
-        <v>62.12121212121212</v>
+        <v>48.93617021276596</v>
       </c>
       <c r="C2" t="n">
-        <v>40.90909090909091</v>
+        <v>36.17021276595745</v>
       </c>
       <c r="D2" t="n">
-        <v>98.48484848484848</v>
+        <v>97.87234042553192</v>
       </c>
       <c r="E2" t="n">
-        <v>37.87878787878788</v>
+        <v>29.78723404255319</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>60.56338028169014</v>
+        <v>53.48837209302325</v>
       </c>
       <c r="B3" t="n">
         <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>43.66197183098591</v>
+        <v>37.2093023255814</v>
       </c>
       <c r="D3" t="n">
-        <v>67.6056338028169</v>
+        <v>62.7906976744186</v>
       </c>
       <c r="E3" t="n">
-        <v>36.61971830985916</v>
+        <v>30.23255813953488</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>32.91139240506329</v>
+        <v>34.69387755102041</v>
       </c>
       <c r="B4" t="n">
-        <v>29.11392405063291</v>
+        <v>32.6530612244898</v>
       </c>
       <c r="C4" t="n">
         <v>100</v>
       </c>
       <c r="D4" t="n">
-        <v>40.50632911392405</v>
+        <v>44.89795918367347</v>
       </c>
       <c r="E4" t="n">
-        <v>31.64556962025317</v>
+        <v>36.73469387755102</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>77.17391304347827</v>
+        <v>68.65671641791045</v>
       </c>
       <c r="B5" t="n">
-        <v>51.08695652173913</v>
+        <v>40.29850746268657</v>
       </c>
       <c r="C5" t="n">
-        <v>36.95652173913043</v>
+        <v>32.83582089552239</v>
       </c>
       <c r="D5" t="n">
         <v>100</v>
       </c>
       <c r="E5" t="n">
-        <v>33.69565217391305</v>
+        <v>26.86567164179105</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>32.7683615819209</v>
+        <v>26.41509433962264</v>
       </c>
       <c r="B6" t="n">
-        <v>27.68361581920904</v>
+        <v>24.52830188679245</v>
       </c>
       <c r="C6" t="n">
-        <v>29.37853107344633</v>
+        <v>33.9622641509434</v>
       </c>
       <c r="D6" t="n">
-        <v>35.02824858757062</v>
+        <v>33.9622641509434</v>
       </c>
       <c r="E6" t="n">
         <v>100</v>

</xml_diff>